<commit_message>
testing multicurve multi instrument, adding more curve types
</commit_message>
<xml_diff>
--- a/testSwap.xlsx
+++ b/testSwap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jennifer Ma\Documents\2019-2020\2020-winter\internship\xll12-master\xll12-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6D5E15D-095F-4645-A463-F641A5984DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56891799-01BB-4CD5-8E8C-E4B0D1EBC465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DC1CCCBD-849E-4E2E-9BDB-607B71FC5278}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,30 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t xml:space="preserve"> 1, 2, 5, 10, 20 </t>
   </si>
@@ -416,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F871DB27-7551-43C3-98FD-E501A1D562B1}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -442,8 +419,17 @@
       <c r="C2">
         <v>-1E-3</v>
       </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -457,13 +443,13 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -473,12 +459,17 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="H4" cm="1">
-        <f t="array" ref="H4:H8">_xll.XLL.swapTest.multi(A2:C6,E3:G3)</f>
-        <v>4.7793927597052557</v>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10</v>
       </c>
@@ -488,11 +479,17 @@
       <c r="C5">
         <v>0.01</v>
       </c>
-      <c r="H5">
-        <v>7.6105940721892642</v>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
@@ -502,42 +499,14 @@
       <c r="C6">
         <v>1E-3</v>
       </c>
-      <c r="E6" cm="1">
-        <f t="array" ref="E6">_xll.XLL.swapTest(A2:C2)</f>
-        <v>4.7793927597052557</v>
-      </c>
-      <c r="H6">
-        <v>13.952780167959688</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E7" cm="1">
-        <f t="array" ref="E7">_xll.XLL.swapTest(A3:C3)</f>
-        <v>7.6105940721892642</v>
-      </c>
-      <c r="H7">
-        <v>47.246171402897403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E8" cm="1">
-        <f t="array" ref="E8">_xll.XLL.swapTest(A4:C4)</f>
-        <v>13.952780167959688</v>
-      </c>
-      <c r="H8">
-        <v>64.5087155106891</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E9" cm="1">
-        <f t="array" ref="E9">_xll.XLL.swapTest(A5:C5)</f>
-        <v>47.246171402897403</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E10" cm="1">
-        <f t="array" ref="E10">_xll.XLL.swapTest(A6:C6)</f>
-        <v>64.5087155106891</v>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>